<commit_message>
#5 NamedThing only schema
</commit_message>
<xml_diff>
--- a/project/excel/monterey_schema.xlsx
+++ b/project/excel/monterey_schema.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Person" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="PersonCollection" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -443,91 +441,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>primary_email</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>birth_date</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>age_in_years</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>vital_status</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>entries</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
#7 upper classes, all rooted
</commit_message>
<xml_diff>
--- a/project/excel/monterey_schema.xlsx
+++ b/project/excel/monterey_schema.xlsx
@@ -8,6 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="MaterialOrData" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="MaterialEntity" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="DataEntity" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="PlannedProcess" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -441,4 +445,158 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
input/output ranges and types
</commit_message>
<xml_diff>
--- a/project/excel/monterey_schema.xlsx
+++ b/project/excel/monterey_schema.xlsx
@@ -7,11 +7,13 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="MaterialOrData" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="MaterialEntity" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="DataEntity" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="PlannedProcess" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="MaterialOrData" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="MaterialEntity" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="DataEntity" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Database" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="MaterialProcessing" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="DataProcessing" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="DataGeneration" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,6 +443,11 @@
           <t>description</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -453,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +484,11 @@
           <t>description</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -489,7 +501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,6 +525,11 @@
           <t>description</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -525,7 +542,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,6 +566,11 @@
           <t>description</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -561,7 +583,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,6 +617,113 @@
           <t>description</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>